<commit_message>
Update std Excel and JSON file for catalysis schema
</commit_message>
<xml_diff>
--- a/test/standard_catalysis_excel_schema.xlsx
+++ b/test/standard_catalysis_excel_schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nukp/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nukp/Downloads/CorsinConnecter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9F1FC8-05F6-ED44-8E6D-4A7A98DA4C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C247092-6EDE-DC49-9C8B-4959EF94C59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16480" yWindow="4400" windowWidth="59500" windowHeight="26300" xr2:uid="{1A6D523C-FE67-4F3F-AA9B-E9FEE83DA8F2}"/>
+    <workbookView xWindow="2920" yWindow="2500" windowWidth="65880" windowHeight="26300" xr2:uid="{1A6D523C-FE67-4F3F-AA9B-E9FEE83DA8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="2" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="481">
   <si>
     <t>Metadata</t>
   </si>
@@ -307,15 +307,9 @@
     <t>Water</t>
   </si>
   <si>
-    <t>hasCatholyte-hasSolvent-hasConstituent</t>
-  </si>
-  <si>
     <t>Catholyte solvent A volume fraction</t>
   </si>
   <si>
-    <t>hasCatholyte-hasSolvent-hasConstituent-hasMeasuredProperty-VolumeFraction</t>
-  </si>
-  <si>
     <t>Catholyte solvent B</t>
   </si>
   <si>
@@ -334,18 +328,12 @@
     <t>PotassiumChloride</t>
   </si>
   <si>
-    <t>hasCatholyte-hasSolute-hasConstituent</t>
-  </si>
-  <si>
     <t xml:space="preserve">Catholyte solute A molarity </t>
   </si>
   <si>
     <t>mol/L</t>
   </si>
   <si>
-    <t>hasCatholyte-hasSolute-hasConstituent-hasMeasuredProperty-AmountConcentration</t>
-  </si>
-  <si>
     <t>Catholyte solute B</t>
   </si>
   <si>
@@ -424,15 +412,9 @@
     <t>Catholyte solvent A manufacturer</t>
   </si>
   <si>
-    <t>hasCatholyte-hasSolvent-schema:manufacturer</t>
-  </si>
-  <si>
     <t>Catholyte solvent A manufacturer product ID</t>
   </si>
   <si>
-    <t>hasCatholyte-hasSolvent-schema:productID</t>
-  </si>
-  <si>
     <t>Catholyte solvent B manufacturer</t>
   </si>
   <si>
@@ -442,15 +424,9 @@
     <t>Catholyte solute A manufacturer</t>
   </si>
   <si>
-    <t>hasCatholyte-hasSolute-schema:manufacturer</t>
-  </si>
-  <si>
     <t>Catholyte solute A manufacturer productD</t>
   </si>
   <si>
-    <t>hasCatholyte-hasSolute-schema:productID</t>
-  </si>
-  <si>
     <t>Catholyte solute B manufacturer</t>
   </si>
   <si>
@@ -463,15 +439,9 @@
     <t>Anolyte solvent A</t>
   </si>
   <si>
-    <t>hasAnolyte-hasSolvent-hasConstituent</t>
-  </si>
-  <si>
     <t>Anolyte solvent A volume fraction</t>
   </si>
   <si>
-    <t>hasAnolyte-hasSolvent-hasConstituent-hasMeasuredProperty-VolumeFraction</t>
-  </si>
-  <si>
     <t>Anolyte solvent B</t>
   </si>
   <si>
@@ -481,15 +451,9 @@
     <t>Anolyte solute A</t>
   </si>
   <si>
-    <t>hasAnolyte-hasSolute-hasConstituent</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anolyte solute A molarity </t>
   </si>
   <si>
-    <t>hasAnolyte-hasSolute-hasConstituent-hasMeasuredProperty-AmountConcentration</t>
-  </si>
-  <si>
     <t>Anolyte solute B</t>
   </si>
   <si>
@@ -991,9 +955,6 @@
     <t>hasPositiveElectrode-hasCoating-hasElectrolyte</t>
   </si>
   <si>
-    <t>hasPositiveElectrode-hasCoating-hasElectrolyte-hasConstituent</t>
-  </si>
-  <si>
     <t>hasPositiveElectrode-hasCoating-hasActiveMaterial</t>
   </si>
   <si>
@@ -1033,9 +994,6 @@
     <t>Positive electrode coating electrolyte type</t>
   </si>
   <si>
-    <t>hasPositiveElectrode-hasCoating-hasElectrolyte-hasConstituent-hasMeasuredProperty-MassFraction</t>
-  </si>
-  <si>
     <t>Positive electrode coating electrolyte material A</t>
   </si>
   <si>
@@ -1171,18 +1129,6 @@
     <t>18x_Ti</t>
   </si>
   <si>
-    <t>hasNegativeElectrode-hasSubstrate_schema:manufacturer</t>
-  </si>
-  <si>
-    <t>hasNegativeElectrode-hasSubstrate_schema:productID</t>
-  </si>
-  <si>
-    <t>hasNegativeElectrode-hasCoating_hasActiveMaterial-schema:manufacturer</t>
-  </si>
-  <si>
-    <t>hasNegativeElectrode-hasCoating_hasActiveMaterial-schema:productID</t>
-  </si>
-  <si>
     <t>Negative electrode coating active material manufacturer</t>
   </si>
   <si>
@@ -1213,24 +1159,12 @@
     <t>Negative electrode gas pressure</t>
   </si>
   <si>
-    <t>hasPositiveElectrode-hasGasFlow-hasConstituent</t>
-  </si>
-  <si>
-    <t>hasPositiveElectrode-hasGasFlow-hasConstituent-MeasuredProperty-VolumeFraction</t>
-  </si>
-  <si>
     <t>hasPositiveElectrode-hasGasFlow-hasMeasuredProperty-VolumeFlowRate</t>
   </si>
   <si>
     <t>hasPositiveElectrode-hasGasFlow-hasMeasuredProperty-Pressure</t>
   </si>
   <si>
-    <t>hasNegativeElectrode-hasGasFlow-hasConstituent</t>
-  </si>
-  <si>
-    <t>hasNegativeElectrode-hasGasFlow-hasConstituent-MeasuredProperty-VolumeFraction</t>
-  </si>
-  <si>
     <t>hasNegativeElectrode-hasGasFlow-hasMeasuredProperty-VolumeFlowRate</t>
   </si>
   <si>
@@ -1399,9 +1333,6 @@
     <t>01/05/2026</t>
   </si>
   <si>
-    <t>BattINFO CoinCellSchema version</t>
-  </si>
-  <si>
     <t>unit:MilliL-PER-MIN</t>
   </si>
   <si>
@@ -1469,6 +1400,129 @@
   </si>
   <si>
     <t>hasComponentE-type|AnolyteTank-hasMeasuredProperty-Volume</t>
+  </si>
+  <si>
+    <t>hasNegativeElectrode-hasSubstrate-schema:manufacturer</t>
+  </si>
+  <si>
+    <t>hasNegativeElectrode-hasSubstrate-schema:productID</t>
+  </si>
+  <si>
+    <t>hasNegativeElectrode-hasCoating-hasActiveMaterial-schema:manufacturer</t>
+  </si>
+  <si>
+    <t>hasNegativeElectrode-hasCoating-hasActiveMaterial-schema:productID</t>
+  </si>
+  <si>
+    <t>hasPositiveElectrode-hasCoating-hasElectrolyte-hasConstituentA</t>
+  </si>
+  <si>
+    <t>hasPositiveElectrode-hasCoating-hasElectrolyte-hasConstituentA-hasMeasuredProperty-MassFraction</t>
+  </si>
+  <si>
+    <t>hasPositiveElectrode-hasCoating-hasElectrolyte-hasConstituentB</t>
+  </si>
+  <si>
+    <t>hasPositiveElectrode-hasCoating-hasElectrolyte-hasConstituentB-hasMeasuredProperty-MassFraction</t>
+  </si>
+  <si>
+    <t>hasPositiveElectrode-hasGasFlow-hasConstituentA</t>
+  </si>
+  <si>
+    <t>hasPositiveElectrode-hasGasFlow-hasConstituentA-MeasuredProperty-VolumeFraction</t>
+  </si>
+  <si>
+    <t>hasPositiveElectrode-hasGasFlow-hasConstituentB</t>
+  </si>
+  <si>
+    <t>hasPositiveElectrode-hasGasFlow-hasConstituentB-MeasuredProperty-VolumeFraction</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolvent-hasConstituentA</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolvent-hasConstituentA-hasMeasuredProperty-VolumeFraction</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolvent-hasConstituentB</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolvent-hasConstituentB-hasMeasuredProperty-VolumeFraction</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolute-hasConstituentA</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolute-hasConstituentA-hasMeasuredProperty-AmountConcentration</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolute-hasConstituentB</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolute-hasConstituentB-hasMeasuredProperty-AmountConcentration</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolventA-schema:manufacturer</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolventA-schema:productID</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolventB-schema:manufacturer</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSolventB-schema:productID</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSoluteA-schema:manufacturer</t>
+  </si>
+  <si>
+    <t>hasCatholyte-hasSoluteA-schema:productID</t>
+  </si>
+  <si>
+    <t>hasNegativeElectrode-hasGasFlow-hasConstituentA</t>
+  </si>
+  <si>
+    <t>hasNegativeElectrode-hasGasFlow-hasConstituentA-MeasuredProperty-VolumeFraction</t>
+  </si>
+  <si>
+    <t>hasNegativeElectrode-hasGasFlow-hasConstituentB</t>
+  </si>
+  <si>
+    <t>hasNegativeElectrode-hasGasFlow-hasConstituentB-MeasuredProperty-VolumeFraction</t>
+  </si>
+  <si>
+    <t>hasAnolyte-hasSolvent-hasConstituentA</t>
+  </si>
+  <si>
+    <t>hasAnolyte-hasSolvent-hasConstituentA-hasMeasuredProperty-VolumeFraction</t>
+  </si>
+  <si>
+    <t>hasAnolyte-hasSolvent-hasConstituentB</t>
+  </si>
+  <si>
+    <t>hasAnolyte-hasSolvent-hasConstituentB-hasMeasuredProperty-VolumeFraction</t>
+  </si>
+  <si>
+    <t>hasAnolyte-hasSolute-hasConstituentA</t>
+  </si>
+  <si>
+    <t>hasAnolyte-hasSolute-hasConstituentA-hasMeasuredProperty-AmountConcentration</t>
+  </si>
+  <si>
+    <t>hasAnolyte-hasSolute-hasConstituentB</t>
+  </si>
+  <si>
+    <t>hasAnolyte-hasSolute-hasConstituentB-hasMeasuredProperty-AmountConcentration</t>
+  </si>
+  <si>
+    <t>hasComponentB-schema:manufacturer</t>
+  </si>
+  <si>
+    <t>hasComponentB-schema:productID</t>
+  </si>
+  <si>
+    <t>Schema version</t>
   </si>
 </sst>
 </file>
@@ -1671,7 +1725,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1818,6 +1872,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2279,8 +2336,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:KA166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B133" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2288,7 +2345,7 @@
     <col min="1" max="1" width="74.796875" style="2" customWidth="1"/>
     <col min="2" max="2" width="35" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="157.796875" style="2" customWidth="1"/>
     <col min="6" max="6" width="67" style="12" customWidth="1"/>
     <col min="7" max="7" width="46.19921875" style="2" customWidth="1"/>
@@ -2330,7 +2387,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>430</v>
+        <v>408</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -2370,7 +2427,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>438</v>
+        <v>416</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -2427,7 +2484,7 @@
     </row>
     <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
-        <v>439</v>
+        <v>480</v>
       </c>
       <c r="B8" s="36">
         <v>0.1</v>
@@ -2490,7 +2547,7 @@
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>25</v>
@@ -2507,10 +2564,10 @@
     </row>
     <row r="13" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>8</v>
@@ -2519,7 +2576,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="2"/>
@@ -2620,7 +2677,7 @@
     </row>
     <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>33</v>
@@ -2632,12 +2689,12 @@
         <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B15" s="6">
         <v>280</v>
@@ -2649,7 +2706,7 @@
         <v>21</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="2"/>
@@ -2750,7 +2807,7 @@
     </row>
     <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>29</v>
@@ -2762,12 +2819,12 @@
         <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>30</v>
@@ -2779,7 +2836,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="2"/>
@@ -2880,7 +2937,7 @@
     </row>
     <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="B18" s="4">
         <v>0.5</v>
@@ -2892,12 +2949,12 @@
         <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="B19" s="6">
         <v>90</v>
@@ -2909,7 +2966,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="2"/>
@@ -3010,7 +3067,7 @@
     </row>
     <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>33</v>
@@ -3022,12 +3079,12 @@
         <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="B21" s="6">
         <v>6</v>
@@ -3039,7 +3096,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="2"/>
@@ -3140,7 +3197,7 @@
     </row>
     <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>34</v>
@@ -3152,15 +3209,15 @@
         <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>8</v>
@@ -3169,7 +3226,7 @@
         <v>9</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>303</v>
+        <v>444</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="2"/>
@@ -3270,7 +3327,7 @@
     </row>
     <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="B24" s="4">
         <v>2</v>
@@ -3282,15 +3339,15 @@
         <v>9</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>317</v>
+        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>8</v>
@@ -3299,7 +3356,7 @@
         <v>9</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>303</v>
+        <v>446</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="2"/>
@@ -3400,7 +3457,7 @@
     </row>
     <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="B26" s="4">
         <v>2</v>
@@ -3412,12 +3469,12 @@
         <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>317</v>
+        <v>447</v>
       </c>
     </row>
     <row r="27" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="B27" s="6">
         <v>0.5</v>
@@ -3429,7 +3486,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="2"/>
@@ -3540,7 +3597,7 @@
     </row>
     <row r="29" spans="1:101" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="B29" s="4">
         <v>35</v>
@@ -3552,30 +3609,30 @@
         <v>36</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:101" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="B30" s="6">
         <v>2.5</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>8</v>
+        <v>242</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>36</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:101" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>37</v>
@@ -3584,7 +3641,7 @@
         <v>36</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:101" x14ac:dyDescent="0.2">
@@ -3634,7 +3691,7 @@
     </row>
     <row r="35" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>44</v>
@@ -3646,12 +3703,12 @@
         <v>36</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>45</v>
@@ -3663,13 +3720,13 @@
         <v>36</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="F36" s="19"/>
     </row>
     <row r="37" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>46</v>
@@ -3681,12 +3738,12 @@
         <v>36</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>47</v>
@@ -3698,13 +3755,13 @@
         <v>36</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>48</v>
@@ -3716,12 +3773,12 @@
         <v>36</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>49</v>
@@ -3733,7 +3790,7 @@
         <v>36</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="F40" s="19"/>
     </row>
@@ -3749,10 +3806,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>8</v>
@@ -3766,10 +3823,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>8</v>
@@ -3778,13 +3835,13 @@
         <v>9</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>52</v>
@@ -3796,12 +3853,12 @@
         <v>9</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="B45" s="10">
         <v>20</v>
@@ -3813,16 +3870,16 @@
         <v>21</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>8</v>
@@ -3831,12 +3888,12 @@
         <v>9</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>53</v>
@@ -3848,13 +3905,13 @@
         <v>9</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="B48" s="4">
         <v>0.5</v>
@@ -3881,7 +3938,7 @@
     </row>
     <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B50" s="4">
         <v>50</v>
@@ -3893,12 +3950,12 @@
         <v>36</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="B51" s="10">
         <v>0</v>
@@ -3910,13 +3967,13 @@
         <v>36</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="F51" s="21"/>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>28</v>
@@ -3960,7 +4017,7 @@
         <v>61</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>8</v>
@@ -3975,10 +4032,10 @@
     </row>
     <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>8</v>
@@ -3987,12 +4044,12 @@
         <v>36</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>363</v>
+        <v>440</v>
       </c>
     </row>
     <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="B57" s="10">
         <v>1000214960</v>
@@ -4004,16 +4061,16 @@
         <v>36</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>364</v>
+        <v>441</v>
       </c>
       <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>8</v>
@@ -4022,12 +4079,12 @@
         <v>36</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>365</v>
+        <v>442</v>
       </c>
     </row>
     <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10" t="s">
@@ -4037,7 +4094,7 @@
         <v>36</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>366</v>
+        <v>443</v>
       </c>
       <c r="F59" s="21"/>
     </row>
@@ -4065,7 +4122,7 @@
         <v>9</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>377</v>
+        <v>448</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -4082,7 +4139,7 @@
         <v>9</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>378</v>
+        <v>449</v>
       </c>
       <c r="F62" s="15"/>
     </row>
@@ -4100,7 +4157,7 @@
         <v>9</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>377</v>
+        <v>450</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -4117,7 +4174,7 @@
         <v>9</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>378</v>
+        <v>451</v>
       </c>
       <c r="F64" s="15"/>
     </row>
@@ -4135,24 +4192,24 @@
         <v>9</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
     </row>
     <row r="66" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="B66" s="11">
         <v>1</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="D66" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="F66" s="15"/>
     </row>
@@ -4180,12 +4237,12 @@
         <v>9</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>75</v>
+        <v>452</v>
       </c>
     </row>
     <row r="69" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="11">
         <v>100</v>
@@ -4197,30 +4254,30 @@
         <v>9</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>77</v>
+        <v>453</v>
       </c>
       <c r="F69" s="15"/>
     </row>
     <row r="70" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>75</v>
+        <v>454</v>
       </c>
     </row>
     <row r="71" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B71" s="11">
         <v>0</v>
@@ -4229,19 +4286,19 @@
         <v>32</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>77</v>
+        <v>455</v>
       </c>
       <c r="F71" s="15"/>
     </row>
     <row r="72" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>8</v>
@@ -4250,24 +4307,24 @@
         <v>9</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>84</v>
+        <v>456</v>
       </c>
     </row>
     <row r="73" spans="1:287" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B73" s="11">
         <v>1</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>87</v>
+        <v>457</v>
       </c>
       <c r="F73" s="15"/>
       <c r="G73" s="2"/>
@@ -4554,7 +4611,7 @@
     </row>
     <row r="74" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>8</v>
@@ -4563,45 +4620,45 @@
         <v>36</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>84</v>
+        <v>458</v>
       </c>
     </row>
     <row r="75" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B75" s="13"/>
       <c r="C75" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>87</v>
+        <v>459</v>
       </c>
       <c r="F75" s="15"/>
     </row>
     <row r="76" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B76" s="4">
         <v>100</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B77" s="64">
         <v>5</v>
@@ -4613,30 +4670,30 @@
         <v>36</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F77" s="15"/>
     </row>
     <row r="78" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B78" s="43">
         <v>1</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A79" s="54" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B79" s="55"/>
       <c r="C79" s="52"/>
@@ -4646,77 +4703,77 @@
     </row>
     <row r="80" spans="1:287" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B80" s="11">
         <v>8</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D80" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F80" s="15"/>
     </row>
     <row r="81" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B81" s="56">
+        <v>96</v>
+      </c>
+      <c r="B81" s="69">
         <v>4.5</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>8</v>
+        <v>242</v>
       </c>
       <c r="D81" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B82" s="11">
         <v>1.3</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D82" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F82" s="15"/>
     </row>
     <row r="83" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B83" s="56">
         <v>25</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D83" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E83" s="57" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="54" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B84" s="55"/>
       <c r="C84" s="52"/>
@@ -4726,7 +4783,7 @@
     </row>
     <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>8</v>
@@ -4735,12 +4792,12 @@
         <v>36</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="11" t="s">
@@ -4750,13 +4807,13 @@
         <v>36</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F86" s="15"/>
     </row>
     <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="4" t="s">
@@ -4766,12 +4823,12 @@
         <v>36</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>114</v>
+        <v>460</v>
       </c>
     </row>
     <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B88" s="14"/>
       <c r="C88" s="11" t="s">
@@ -4781,13 +4838,13 @@
         <v>36</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>116</v>
+        <v>461</v>
       </c>
       <c r="F88" s="15"/>
     </row>
     <row r="89" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="4" t="s">
@@ -4797,12 +4854,12 @@
         <v>36</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>114</v>
+        <v>462</v>
       </c>
     </row>
     <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="11" t="s">
@@ -4812,13 +4869,13 @@
         <v>36</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>116</v>
+        <v>463</v>
       </c>
       <c r="F90" s="15"/>
     </row>
     <row r="91" spans="1:6" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="4" t="s">
@@ -4828,12 +4885,12 @@
         <v>36</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>120</v>
+        <v>464</v>
       </c>
     </row>
     <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B92" s="14"/>
       <c r="C92" s="11" t="s">
@@ -4843,13 +4900,13 @@
         <v>36</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>122</v>
+        <v>465</v>
       </c>
       <c r="F92" s="15"/>
     </row>
     <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>8</v>
@@ -4858,12 +4915,12 @@
         <v>36</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>120</v>
+        <v>464</v>
       </c>
     </row>
     <row r="94" spans="1:6" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B94" s="11"/>
       <c r="C94" s="11" t="s">
@@ -4873,13 +4930,13 @@
         <v>36</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>122</v>
+        <v>465</v>
       </c>
       <c r="F94" s="15"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="51" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="B95" s="52"/>
       <c r="C95" s="52"/>
@@ -4889,7 +4946,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>8</v>
@@ -4898,12 +4955,12 @@
         <v>36</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>381</v>
+        <v>466</v>
       </c>
     </row>
     <row r="97" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A97" s="13" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="B97" s="11"/>
       <c r="C97" s="11" t="s">
@@ -4913,13 +4970,13 @@
         <v>36</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>382</v>
+        <v>467</v>
       </c>
       <c r="F97" s="15"/>
     </row>
     <row r="98" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>8</v>
@@ -4928,12 +4985,12 @@
         <v>36</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>381</v>
+        <v>468</v>
       </c>
     </row>
     <row r="99" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="B99" s="11"/>
       <c r="C99" s="11" t="s">
@@ -4943,13 +5000,13 @@
         <v>36</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>382</v>
+        <v>469</v>
       </c>
       <c r="F99" s="15"/>
     </row>
     <row r="100" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>71</v>
@@ -4958,28 +5015,28 @@
         <v>36</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
     </row>
     <row r="101" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="B101" s="11"/>
       <c r="C101" s="11" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="D101" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="F101" s="15"/>
     </row>
     <row r="102" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A102" s="51" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B102" s="52"/>
       <c r="C102" s="52"/>
@@ -4989,7 +5046,7 @@
     </row>
     <row r="103" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>74</v>
@@ -5001,12 +5058,12 @@
         <v>9</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>127</v>
+        <v>470</v>
       </c>
     </row>
     <row r="104" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B104" s="11">
         <v>100</v>
@@ -5018,30 +5075,30 @@
         <v>9</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>129</v>
+        <v>471</v>
       </c>
       <c r="F104" s="15"/>
     </row>
     <row r="105" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>127</v>
+        <v>472</v>
       </c>
     </row>
     <row r="106" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B106" s="11">
         <v>0</v>
@@ -5050,19 +5107,19 @@
         <v>32</v>
       </c>
       <c r="D106" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E106" s="13" t="s">
-        <v>129</v>
+        <v>473</v>
       </c>
       <c r="F106" s="15"/>
     </row>
     <row r="107" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>8</v>
@@ -5071,24 +5128,24 @@
         <v>9</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>133</v>
+        <v>474</v>
       </c>
     </row>
     <row r="108" spans="1:287" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="13" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B108" s="11">
         <v>1</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E108" s="13" t="s">
-        <v>135</v>
+        <v>475</v>
       </c>
       <c r="F108" s="15"/>
       <c r="G108" s="2"/>
@@ -5375,7 +5432,7 @@
     </row>
     <row r="109" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>8</v>
@@ -5384,45 +5441,45 @@
         <v>36</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>133</v>
+        <v>476</v>
       </c>
     </row>
     <row r="110" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B110" s="11"/>
       <c r="C110" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D110" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E110" s="13" t="s">
-        <v>135</v>
+        <v>477</v>
       </c>
       <c r="F110" s="15"/>
     </row>
     <row r="111" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B111" s="4">
         <v>100</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="D111" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B112" s="64">
         <v>5</v>
@@ -5434,30 +5491,30 @@
         <v>36</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F112" s="15"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B113" s="43">
         <v>1</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="D113" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="54" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B114" s="55"/>
       <c r="C114" s="52"/>
@@ -5467,25 +5524,25 @@
     </row>
     <row r="115" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A115" s="13" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="B115" s="11">
         <v>8</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D115" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
       <c r="F115" s="15"/>
     </row>
     <row r="116" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="B116" s="56">
         <v>4.5</v>
@@ -5497,47 +5554,47 @@
         <v>36</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
     </row>
     <row r="117" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A117" s="13" t="s">
-        <v>387</v>
+        <v>365</v>
       </c>
       <c r="B117" s="11">
         <v>1.3</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D117" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
       <c r="F117" s="15"/>
     </row>
     <row r="118" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
       <c r="B118" s="56">
         <v>25</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D118" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E118" s="57" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="54" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B119" s="55"/>
       <c r="C119" s="52"/>
@@ -5547,7 +5604,7 @@
     </row>
     <row r="120" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>8</v>
@@ -5556,12 +5613,12 @@
         <v>36</v>
       </c>
       <c r="E120" s="12" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="121" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A121" s="13" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B121" s="14"/>
       <c r="C121" s="11" t="s">
@@ -5571,13 +5628,13 @@
         <v>36</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="F121" s="15"/>
     </row>
     <row r="122" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B122" s="7"/>
       <c r="C122" s="4" t="s">
@@ -5587,12 +5644,12 @@
         <v>36</v>
       </c>
       <c r="E122" s="12" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B123" s="14"/>
       <c r="C123" s="11" t="s">
@@ -5602,13 +5659,13 @@
         <v>36</v>
       </c>
       <c r="E123" s="13" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F123" s="15"/>
     </row>
     <row r="124" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B124" s="7"/>
       <c r="C124" s="4" t="s">
@@ -5618,12 +5675,12 @@
         <v>36</v>
       </c>
       <c r="E124" s="12" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A125" s="13" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B125" s="14"/>
       <c r="C125" s="11" t="s">
@@ -5633,13 +5690,13 @@
         <v>36</v>
       </c>
       <c r="E125" s="13" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F125" s="15"/>
     </row>
     <row r="126" spans="1:6" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="4" t="s">
@@ -5649,12 +5706,12 @@
         <v>36</v>
       </c>
       <c r="E126" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="127" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A127" s="13" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="B127" s="14"/>
       <c r="C127" s="11" t="s">
@@ -5664,13 +5721,13 @@
         <v>36</v>
       </c>
       <c r="E127" s="13" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F127" s="15"/>
     </row>
     <row r="128" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>8</v>
@@ -5679,12 +5736,12 @@
         <v>36</v>
       </c>
       <c r="E128" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="129" spans="1:287" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A129" s="13" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B129" s="11"/>
       <c r="C129" s="11" t="s">
@@ -5694,13 +5751,13 @@
         <v>36</v>
       </c>
       <c r="E129" s="13" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F129" s="15"/>
     </row>
     <row r="130" spans="1:287" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A130" s="58" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B130" s="59"/>
       <c r="C130" s="59"/>
@@ -5710,10 +5767,10 @@
     </row>
     <row r="131" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="35" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="B131" s="36" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C131" s="36" t="s">
         <v>8</v>
@@ -5722,7 +5779,7 @@
         <v>9</v>
       </c>
       <c r="E131" s="35" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F131" s="37"/>
       <c r="G131" s="2"/>
@@ -6009,10 +6066,10 @@
     </row>
     <row r="132" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>8</v>
@@ -6021,15 +6078,15 @@
         <v>36</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="133" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="35" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
       <c r="B133" s="36" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="C133" s="36" t="s">
         <v>8</v>
@@ -6038,7 +6095,7 @@
         <v>9</v>
       </c>
       <c r="E133" s="35" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="F133" s="37"/>
       <c r="G133" s="2"/>
@@ -6325,10 +6382,10 @@
     </row>
     <row r="134" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>8</v>
@@ -6337,16 +6394,16 @@
         <v>9</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
       <c r="F134" s="2"/>
     </row>
     <row r="135" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="35" t="s">
-        <v>402</v>
+        <v>380</v>
       </c>
       <c r="B135" s="36" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C135" s="36" t="s">
         <v>8</v>
@@ -6355,7 +6412,7 @@
         <v>9</v>
       </c>
       <c r="E135" s="35" t="s">
-        <v>405</v>
+        <v>383</v>
       </c>
       <c r="F135" s="37"/>
       <c r="G135" s="2"/>
@@ -6642,7 +6699,7 @@
     </row>
     <row r="136" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>396</v>
+        <v>374</v>
       </c>
       <c r="B136" s="4">
         <v>500</v>
@@ -6654,16 +6711,16 @@
         <v>21</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="F136" s="2"/>
     </row>
     <row r="137" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="35" t="s">
-        <v>397</v>
+        <v>375</v>
       </c>
       <c r="B137" s="36" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="C137" s="36" t="s">
         <v>8</v>
@@ -6672,7 +6729,7 @@
         <v>36</v>
       </c>
       <c r="E137" s="35" t="s">
-        <v>410</v>
+        <v>388</v>
       </c>
       <c r="F137" s="37"/>
       <c r="G137" s="2"/>
@@ -6959,10 +7016,10 @@
     </row>
     <row r="138" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>8</v>
@@ -6971,16 +7028,16 @@
         <v>36</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>412</v>
+        <v>390</v>
       </c>
       <c r="F138" s="2"/>
     </row>
     <row r="139" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="35" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="B139" s="36" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C139" s="36" t="s">
         <v>8</v>
@@ -6989,7 +7046,7 @@
         <v>36</v>
       </c>
       <c r="E139" s="35" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="F139" s="37"/>
       <c r="G139" s="2"/>
@@ -7276,7 +7333,7 @@
     </row>
     <row r="140" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
       <c r="B140" s="4">
         <v>500</v>
@@ -7288,13 +7345,13 @@
         <v>36</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>413</v>
+        <v>391</v>
       </c>
       <c r="F140" s="2"/>
     </row>
     <row r="141" spans="1:287" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A141" s="58" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B141" s="59"/>
       <c r="C141" s="59"/>
@@ -7304,19 +7361,19 @@
     </row>
     <row r="142" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="35" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B142" s="36">
         <v>8</v>
       </c>
       <c r="C142" s="36" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D142" s="37" t="s">
         <v>36</v>
       </c>
       <c r="E142" s="35" t="s">
-        <v>414</v>
+        <v>392</v>
       </c>
       <c r="F142" s="37"/>
       <c r="G142" s="2"/>
@@ -7603,24 +7660,24 @@
     </row>
     <row r="143" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B143" s="4">
         <v>8</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D143" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
     </row>
     <row r="144" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A144" s="58" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B144" s="59"/>
       <c r="C144" s="59"/>
@@ -7630,7 +7687,7 @@
     </row>
     <row r="145" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="35" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B145" s="36" t="s">
         <v>48</v>
@@ -7642,7 +7699,7 @@
         <v>36</v>
       </c>
       <c r="E145" s="35" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="F145" s="37"/>
       <c r="G145" s="2"/>
@@ -7929,7 +7986,7 @@
     </row>
     <row r="146" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>49</v>
@@ -7941,15 +7998,15 @@
         <v>36</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
     </row>
     <row r="147" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="35" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B147" s="36" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C147" s="36" t="s">
         <v>8</v>
@@ -7958,7 +8015,7 @@
         <v>36</v>
       </c>
       <c r="E147" s="35" t="s">
-        <v>453</v>
+        <v>478</v>
       </c>
       <c r="F147" s="37"/>
       <c r="G147" s="2"/>
@@ -8245,10 +8302,10 @@
     </row>
     <row r="148" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>8</v>
@@ -8257,12 +8314,12 @@
         <v>36</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>454</v>
+        <v>479</v>
       </c>
     </row>
     <row r="149" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A149" s="58" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B149" s="59"/>
       <c r="C149" s="59"/>
@@ -8272,10 +8329,10 @@
     </row>
     <row r="150" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="35" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="B150" s="36" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="C150" s="36" t="s">
         <v>8</v>
@@ -8284,7 +8341,7 @@
         <v>9</v>
       </c>
       <c r="E150" s="35" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F150" s="37"/>
       <c r="G150" s="2"/>
@@ -8571,10 +8628,10 @@
     </row>
     <row r="151" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>434</v>
+        <v>412</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>8</v>
@@ -8583,24 +8640,24 @@
         <v>9</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="152" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="35" t="s">
-        <v>435</v>
+        <v>413</v>
       </c>
       <c r="B152" s="36">
         <v>4</v>
       </c>
       <c r="C152" s="36" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="D152" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E152" s="35" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
       <c r="F152" s="37"/>
       <c r="G152" s="2"/>
@@ -8887,36 +8944,36 @@
     </row>
     <row r="153" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>426</v>
+        <v>404</v>
       </c>
       <c r="B153" s="4">
         <v>1</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D153" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>455</v>
+        <v>432</v>
       </c>
     </row>
     <row r="154" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="35" t="s">
-        <v>417</v>
+        <v>395</v>
       </c>
       <c r="B154" s="36">
         <v>100</v>
       </c>
       <c r="C154" s="36" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="D154" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E154" s="35" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
       <c r="F154" s="37"/>
       <c r="G154" s="2"/>
@@ -9203,10 +9260,10 @@
     </row>
     <row r="155" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="35" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
       <c r="B155" s="36" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="C155" s="36" t="s">
         <v>8</v>
@@ -9215,7 +9272,7 @@
         <v>36</v>
       </c>
       <c r="E155" s="35" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="F155" s="37"/>
       <c r="G155" s="2"/>
@@ -9502,36 +9559,36 @@
     </row>
     <row r="156" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>418</v>
+        <v>396</v>
       </c>
       <c r="B156" s="4">
         <v>500</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="D156" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
     </row>
     <row r="157" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="35" t="s">
-        <v>436</v>
+        <v>414</v>
       </c>
       <c r="B157" s="36">
         <v>4</v>
       </c>
       <c r="C157" s="36" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="D157" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E157" s="35" t="s">
-        <v>431</v>
+        <v>409</v>
       </c>
       <c r="F157" s="37"/>
       <c r="G157" s="2"/>
@@ -9818,36 +9875,36 @@
     </row>
     <row r="158" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="B158" s="4">
         <v>1</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D158" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
     </row>
     <row r="159" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="35" t="s">
-        <v>419</v>
+        <v>397</v>
       </c>
       <c r="B159" s="36">
         <v>100</v>
       </c>
       <c r="C159" s="36" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="D159" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E159" s="35" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="F159" s="37"/>
       <c r="G159" s="2"/>
@@ -10134,7 +10191,7 @@
     </row>
     <row r="160" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="35" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="B160" s="36"/>
       <c r="C160" s="36" t="s">
@@ -10144,7 +10201,7 @@
         <v>36</v>
       </c>
       <c r="E160" s="35" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="F160" s="37"/>
       <c r="G160" s="2"/>
@@ -10431,36 +10488,36 @@
     </row>
     <row r="161" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
       <c r="B161" s="4">
         <v>500</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="D161" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
     </row>
     <row r="162" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="35" t="s">
-        <v>437</v>
+        <v>415</v>
       </c>
       <c r="B162" s="36">
         <v>4</v>
       </c>
       <c r="C162" s="36" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="D162" s="37" t="s">
         <v>36</v>
       </c>
       <c r="E162" s="35" t="s">
-        <v>428</v>
+        <v>406</v>
       </c>
       <c r="F162" s="37"/>
       <c r="G162" s="2"/>
@@ -10747,7 +10804,7 @@
     </row>
     <row r="163" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A163" s="61" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B163" s="62"/>
       <c r="C163" s="62"/>
@@ -10757,10 +10814,10 @@
     </row>
     <row r="164" spans="1:287" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>8</v>
@@ -10769,12 +10826,12 @@
         <v>36</v>
       </c>
       <c r="E164" s="12" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="165" spans="1:287" s="35" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A165" s="35" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B165" s="36"/>
       <c r="C165" s="36" t="s">
@@ -10784,7 +10841,7 @@
         <v>36</v>
       </c>
       <c r="E165" s="37" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F165" s="37"/>
       <c r="G165" s="2"/>
@@ -11144,66 +11201,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -11238,57 +11295,57 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B1" s="66" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -11296,7 +11353,7 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -11304,89 +11361,89 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B11" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B13" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B14" s="27"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B15" s="28"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B22" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -11405,10 +11462,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43ECF056-09CF-D34B-89B9-B55BABB0D56E}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -11418,26 +11475,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -11445,23 +11502,23 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -11469,23 +11526,23 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.25">
@@ -11493,79 +11550,79 @@
         <v>28</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B16" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="B19" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -11573,32 +11630,35 @@
         <v>71</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="B21" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="B22" s="67" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="B23" s="67" t="s">
-        <v>451</v>
-      </c>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="B24" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11608,10 +11668,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA002F9-7520-4BAF-85B4-9FA6117747D6}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="A18" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -11623,21 +11683,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -11647,15 +11707,15 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -11665,42 +11725,42 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -11708,7 +11768,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -11716,36 +11776,36 @@
         <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="B17" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B18" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B20" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -11753,68 +11813,68 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="B23" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
@@ -11829,22 +11889,22 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
@@ -11854,22 +11914,22 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
@@ -11879,37 +11939,37 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>416</v>
+        <v>394</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>423</v>
+        <v>401</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
@@ -11919,7 +11979,7 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
@@ -11929,7 +11989,17 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>448</v>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -11943,6 +12013,59 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FolderType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <CultureName xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <IsNotebookLocked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Invited_Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Math_Settings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Has_Leaders_Only_SectionGroup xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Member_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <Distribution_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <AppVersion xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Templates xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <NotebookType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <TeamsChannelId xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Invited_Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Owner xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <LMS_Mappings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <_activity xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100F5BD758A7F2BF742ADB9291A93682A9E" ma:contentTypeVersion="31" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0517f02299b6dbd064809d9c3f869e8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="35345429-01ed-4d83-85b9-6cc21878d784" xmlns:ns4="53f86fb7-11c0-476e-bf8b-57768422e991" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7ff6e993c77c55b2c02ebba747ae01b" ns3:_="" ns4:_="">
     <xsd:import namespace="35345429-01ed-4d83-85b9-6cc21878d784"/>
@@ -12339,59 +12462,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FolderType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <CultureName xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <IsNotebookLocked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Invited_Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Math_Settings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Has_Leaders_Only_SectionGroup xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Member_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <Distribution_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <AppVersion xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Templates xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <NotebookType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <TeamsChannelId xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Invited_Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Owner xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <LMS_Mappings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <_activity xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12402,6 +12472,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D89A20-922B-4399-8A99-02ABCC3D1E33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="35345429-01ed-4d83-85b9-6cc21878d784"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D716C96-A80E-4732-A5D3-9C77E88EE8CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12420,16 +12500,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D89A20-922B-4399-8A99-02ABCC3D1E33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="35345429-01ed-4d83-85b9-6cc21878d784"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E85C156E-EE0C-426A-92B3-CAF84DB17690}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
small changes in Excel
</commit_message>
<xml_diff>
--- a/test/standard_catalysis_excel_schema.xlsx
+++ b/test/standard_catalysis_excel_schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nukp/Downloads/CorsinConnecter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nukp/Documents/Repository/BattInfoConverter-Empa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C247092-6EDE-DC49-9C8B-4959EF94C59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A975084B-C5B8-8547-9A5E-527E6C9D3B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="2500" windowWidth="65880" windowHeight="26300" xr2:uid="{1A6D523C-FE67-4F3F-AA9B-E9FEE83DA8F2}"/>
   </bookViews>
@@ -2336,8 +2336,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:KA166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -12013,6 +12013,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <FolderType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
@@ -12065,7 +12074,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100F5BD758A7F2BF742ADB9291A93682A9E" ma:contentTypeVersion="31" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0517f02299b6dbd064809d9c3f869e8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="35345429-01ed-4d83-85b9-6cc21878d784" xmlns:ns4="53f86fb7-11c0-476e-bf8b-57768422e991" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7ff6e993c77c55b2c02ebba747ae01b" ns3:_="" ns4:_="">
     <xsd:import namespace="35345429-01ed-4d83-85b9-6cc21878d784"/>
@@ -12462,16 +12471,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E85C156E-EE0C-426A-92B3-CAF84DB17690}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D89A20-922B-4399-8A99-02ABCC3D1E33}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -12481,7 +12489,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D716C96-A80E-4732-A5D3-9C77E88EE8CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12498,12 +12506,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E85C156E-EE0C-426A-92B3-CAF84DB17690}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add files for new test, to fix issue with @type and list
</commit_message>
<xml_diff>
--- a/test/standard_catalysis_excel_schema.xlsx
+++ b/test/standard_catalysis_excel_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nukp/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nukp/Downloads/Corsin request Monday 26Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC04F024-D334-DB4E-8821-6FCB26ACECF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF49684-CEB5-ED44-835A-52BAB6047D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14320" yWindow="1880" windowWidth="47980" windowHeight="26000" xr2:uid="{1A6D523C-FE67-4F3F-AA9B-E9FEE83DA8F2}"/>
+    <workbookView xWindow="6180" yWindow="2800" windowWidth="47980" windowHeight="26000" xr2:uid="{1A6D523C-FE67-4F3F-AA9B-E9FEE83DA8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="@Schema" sheetId="2" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="486">
   <si>
     <t>Metadata</t>
   </si>
@@ -473,9 +473,6 @@
   </si>
   <si>
     <t>Membrane A area specific conductivity</t>
-  </si>
-  <si>
-    <t>mS cm2</t>
   </si>
   <si>
     <t>Membrane B area specific conductivity</t>
@@ -2015,11 +2012,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF8DFB"/>
       <color rgb="FF009C4A"/>
       <color rgb="FFFF0000"/>
       <color rgb="FFFF7815"/>
       <color rgb="FF28C840"/>
-      <color rgb="FFFF8DFB"/>
       <color rgb="FFFF00F6"/>
     </mruColors>
   </colors>
@@ -2354,8 +2351,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:KA167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2405,7 +2402,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -2445,7 +2442,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -2502,10 +2499,10 @@
     </row>
     <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>402</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>403</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -2519,7 +2516,7 @@
     </row>
     <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B9" s="36">
         <v>0.1</v>
@@ -2572,7 +2569,7 @@
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -2582,7 +2579,7 @@
     </row>
     <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
@@ -2599,10 +2596,10 @@
     </row>
     <row r="14" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>8</v>
@@ -2611,7 +2608,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="2"/>
@@ -2712,7 +2709,7 @@
     </row>
     <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>32</v>
@@ -2724,12 +2721,12 @@
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B16" s="6">
         <v>280</v>
@@ -2741,7 +2738,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="2"/>
@@ -2842,7 +2839,7 @@
     </row>
     <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>28</v>
@@ -2854,12 +2851,12 @@
         <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>29</v>
@@ -2871,7 +2868,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="2"/>
@@ -2972,7 +2969,7 @@
     </row>
     <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B19" s="4">
         <v>0.5</v>
@@ -2984,12 +2981,12 @@
         <v>9</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B20" s="6">
         <v>90</v>
@@ -3001,7 +2998,7 @@
         <v>9</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="2"/>
@@ -3102,7 +3099,7 @@
     </row>
     <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>32</v>
@@ -3114,12 +3111,12 @@
         <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B22" s="6">
         <v>6</v>
@@ -3131,7 +3128,7 @@
         <v>9</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="2"/>
@@ -3232,7 +3229,7 @@
     </row>
     <row r="23" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>33</v>
@@ -3244,15 +3241,15 @@
         <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="24" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>8</v>
@@ -3261,7 +3258,7 @@
         <v>9</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="2"/>
@@ -3362,7 +3359,7 @@
     </row>
     <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B25" s="4">
         <v>2</v>
@@ -3374,15 +3371,15 @@
         <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="26" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>8</v>
@@ -3391,7 +3388,7 @@
         <v>9</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="2"/>
@@ -3492,7 +3489,7 @@
     </row>
     <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B27" s="4">
         <v>2</v>
@@ -3504,12 +3501,12 @@
         <v>9</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="28" spans="1:101" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B28" s="6">
         <v>0.5</v>
@@ -3521,7 +3518,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="2"/>
@@ -3622,7 +3619,7 @@
     </row>
     <row r="29" spans="1:101" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="39"/>
@@ -3632,7 +3629,7 @@
     </row>
     <row r="30" spans="1:101" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B30" s="4">
         <v>35</v>
@@ -3644,30 +3641,30 @@
         <v>34</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="31" spans="1:101" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B31" s="6">
         <v>2.5</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F31" s="19"/>
     </row>
     <row r="32" spans="1:101" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>35</v>
@@ -3676,12 +3673,12 @@
         <v>34</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="39"/>
@@ -3691,7 +3688,7 @@
     </row>
     <row r="34" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>16</v>
@@ -3703,12 +3700,12 @@
         <v>34</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="35" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>36</v>
@@ -3720,13 +3717,13 @@
         <v>34</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F35" s="19"/>
     </row>
     <row r="36" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>37</v>
@@ -3738,12 +3735,12 @@
         <v>34</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="37" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>38</v>
@@ -3755,13 +3752,13 @@
         <v>34</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>39</v>
@@ -3773,12 +3770,12 @@
         <v>34</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>40</v>
@@ -3790,13 +3787,13 @@
         <v>34</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F39" s="19"/>
     </row>
     <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>41</v>
@@ -3808,12 +3805,12 @@
         <v>34</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>42</v>
@@ -3825,13 +3822,13 @@
         <v>34</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F41" s="19"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
@@ -3841,10 +3838,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>8</v>
@@ -3858,10 +3855,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>8</v>
@@ -3870,13 +3867,13 @@
         <v>9</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>44</v>
@@ -3888,12 +3885,12 @@
         <v>9</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B46" s="10">
         <v>20</v>
@@ -3905,13 +3902,13 @@
         <v>21</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>28</v>
@@ -3923,12 +3920,12 @@
         <v>9</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>45</v>
@@ -3940,13 +3937,13 @@
         <v>9</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B49" s="4">
         <v>0.5</v>
@@ -3958,12 +3955,12 @@
         <v>21</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="50" spans="1:6" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A50" s="47" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B50" s="48"/>
       <c r="C50" s="49"/>
@@ -3973,7 +3970,7 @@
     </row>
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B51" s="4">
         <v>50</v>
@@ -3985,30 +3982,30 @@
         <v>34</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B52" s="10">
         <v>0</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="D52" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F52" s="21"/>
     </row>
     <row r="53" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>27</v>
@@ -4017,12 +4014,12 @@
         <v>34</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="47" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B54" s="48"/>
       <c r="C54" s="49"/>
@@ -4032,7 +4029,7 @@
     </row>
     <row r="55" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>16</v>
@@ -4044,15 +4041,15 @@
         <v>34</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>8</v>
@@ -4061,16 +4058,16 @@
         <v>34</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>8</v>
@@ -4079,12 +4076,12 @@
         <v>34</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B58" s="10">
         <v>1000214960</v>
@@ -4096,16 +4093,16 @@
         <v>34</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F58" s="21"/>
     </row>
     <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>8</v>
@@ -4114,12 +4111,12 @@
         <v>34</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="10" t="s">
@@ -4129,13 +4126,13 @@
         <v>34</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F60" s="21"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="51" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B61" s="52"/>
       <c r="C61" s="52"/>
@@ -4145,7 +4142,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>47</v>
@@ -4157,12 +4154,12 @@
         <v>9</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B63" s="11">
         <v>10</v>
@@ -4174,13 +4171,13 @@
         <v>9</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F63" s="15"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>48</v>
@@ -4192,12 +4189,12 @@
         <v>9</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="65" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B65" s="11">
         <v>90</v>
@@ -4209,13 +4206,13 @@
         <v>9</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F65" s="15"/>
     </row>
     <row r="66" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B66" s="4">
         <v>5</v>
@@ -4227,24 +4224,24 @@
         <v>9</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="67" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B67" s="11">
         <v>1</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D67" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F67" s="15"/>
     </row>
@@ -4272,7 +4269,7 @@
         <v>9</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="70" spans="1:287" x14ac:dyDescent="0.2">
@@ -4289,7 +4286,7 @@
         <v>9</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F70" s="15"/>
     </row>
@@ -4307,7 +4304,7 @@
         <v>56</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="72" spans="1:287" x14ac:dyDescent="0.2">
@@ -4324,7 +4321,7 @@
         <v>56</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F72" s="15"/>
     </row>
@@ -4342,7 +4339,7 @@
         <v>9</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74" spans="1:287" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -4359,7 +4356,7 @@
         <v>9</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F74" s="15"/>
       <c r="G74" s="2"/>
@@ -4655,7 +4652,7 @@
         <v>34</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="76" spans="1:287" x14ac:dyDescent="0.2">
@@ -4670,7 +4667,7 @@
         <v>34</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F76" s="15"/>
     </row>
@@ -4682,7 +4679,7 @@
         <v>100</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D77" s="12" t="s">
         <v>34</v>
@@ -4717,7 +4714,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D79" s="12" t="s">
         <v>34</v>
@@ -4762,7 +4759,7 @@
         <v>4.5</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D82" s="12" t="s">
         <v>34</v>
@@ -4858,7 +4855,7 @@
         <v>34</v>
       </c>
       <c r="E88" s="12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="89" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4873,7 +4870,7 @@
         <v>34</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F89" s="15"/>
     </row>
@@ -4889,7 +4886,7 @@
         <v>34</v>
       </c>
       <c r="E90" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="91" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4904,7 +4901,7 @@
         <v>34</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F91" s="15"/>
     </row>
@@ -4920,7 +4917,7 @@
         <v>34</v>
       </c>
       <c r="E92" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4935,7 +4932,7 @@
         <v>34</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F93" s="15"/>
     </row>
@@ -4950,7 +4947,7 @@
         <v>34</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="95" spans="1:6" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
@@ -4965,13 +4962,13 @@
         <v>34</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F95" s="15"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="51" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B96" s="52"/>
       <c r="C96" s="52"/>
@@ -4981,7 +4978,7 @@
     </row>
     <row r="97" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>8</v>
@@ -4990,12 +4987,12 @@
         <v>34</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="98" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="11" t="s">
@@ -5005,13 +5002,13 @@
         <v>34</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F98" s="15"/>
     </row>
     <row r="99" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>8</v>
@@ -5020,12 +5017,12 @@
         <v>34</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="100" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B100" s="11"/>
       <c r="C100" s="11" t="s">
@@ -5035,13 +5032,13 @@
         <v>34</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F100" s="15"/>
     </row>
     <row r="101" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>49</v>
@@ -5050,22 +5047,22 @@
         <v>34</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="102" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B102" s="11"/>
       <c r="C102" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D102" s="15" t="s">
         <v>34</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F102" s="15"/>
     </row>
@@ -5093,7 +5090,7 @@
         <v>9</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="105" spans="1:287" x14ac:dyDescent="0.2">
@@ -5110,7 +5107,7 @@
         <v>9</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F105" s="15"/>
     </row>
@@ -5128,7 +5125,7 @@
         <v>56</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="107" spans="1:287" x14ac:dyDescent="0.2">
@@ -5145,7 +5142,7 @@
         <v>56</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F107" s="15"/>
     </row>
@@ -5163,7 +5160,7 @@
         <v>9</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="109" spans="1:287" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -5180,7 +5177,7 @@
         <v>9</v>
       </c>
       <c r="E109" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F109" s="15"/>
       <c r="G109" s="2"/>
@@ -5476,7 +5473,7 @@
         <v>34</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="111" spans="1:287" x14ac:dyDescent="0.2">
@@ -5491,7 +5488,7 @@
         <v>34</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F111" s="15"/>
     </row>
@@ -5503,7 +5500,7 @@
         <v>100</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D112" s="12" t="s">
         <v>34</v>
@@ -5538,7 +5535,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D114" s="12" t="s">
         <v>34</v>
@@ -5559,7 +5556,7 @@
     </row>
     <row r="116" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B116" s="11">
         <v>8</v>
@@ -5571,13 +5568,13 @@
         <v>34</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F116" s="15"/>
     </row>
     <row r="117" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B117" s="56">
         <v>4.5</v>
@@ -5589,12 +5586,12 @@
         <v>34</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="118" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B118" s="11">
         <v>1.3</v>
@@ -5606,13 +5603,13 @@
         <v>34</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F118" s="15"/>
     </row>
     <row r="119" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B119" s="56">
         <v>25</v>
@@ -5624,7 +5621,7 @@
         <v>34</v>
       </c>
       <c r="E119" s="57" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -5802,10 +5799,10 @@
     </row>
     <row r="132" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="35" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B132" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C132" s="36" t="s">
         <v>8</v>
@@ -5814,7 +5811,7 @@
         <v>9</v>
       </c>
       <c r="E132" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F132" s="37"/>
       <c r="G132" s="2"/>
@@ -6101,10 +6098,10 @@
     </row>
     <row r="133" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>8</v>
@@ -6113,15 +6110,15 @@
         <v>34</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="134" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="35" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B134" s="36" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C134" s="36" t="s">
         <v>8</v>
@@ -6130,7 +6127,7 @@
         <v>9</v>
       </c>
       <c r="E134" s="35" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F134" s="37"/>
       <c r="G134" s="2"/>
@@ -6417,10 +6414,10 @@
     </row>
     <row r="135" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>8</v>
@@ -6429,16 +6426,16 @@
         <v>9</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F135" s="2"/>
     </row>
     <row r="136" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B136" s="36" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C136" s="36" t="s">
         <v>8</v>
@@ -6447,7 +6444,7 @@
         <v>9</v>
       </c>
       <c r="E136" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F136" s="37"/>
       <c r="G136" s="2"/>
@@ -6734,7 +6731,7 @@
     </row>
     <row r="137" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B137" s="4">
         <v>500</v>
@@ -6746,16 +6743,16 @@
         <v>21</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F137" s="2"/>
     </row>
     <row r="138" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="35" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B138" s="36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C138" s="36" t="s">
         <v>8</v>
@@ -6764,7 +6761,7 @@
         <v>34</v>
       </c>
       <c r="E138" s="35" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F138" s="37"/>
       <c r="G138" s="2"/>
@@ -7051,10 +7048,10 @@
     </row>
     <row r="139" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>8</v>
@@ -7063,16 +7060,16 @@
         <v>34</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F139" s="2"/>
     </row>
     <row r="140" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="35" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B140" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C140" s="36" t="s">
         <v>8</v>
@@ -7081,7 +7078,7 @@
         <v>34</v>
       </c>
       <c r="E140" s="35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F140" s="37"/>
       <c r="G140" s="2"/>
@@ -7368,7 +7365,7 @@
     </row>
     <row r="141" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B141" s="4">
         <v>500</v>
@@ -7380,7 +7377,7 @@
         <v>34</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -7402,13 +7399,13 @@
         <v>8</v>
       </c>
       <c r="C143" s="36" t="s">
-        <v>131</v>
+        <v>72</v>
       </c>
       <c r="D143" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E143" s="35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F143" s="37"/>
       <c r="G143" s="2"/>
@@ -7695,24 +7692,24 @@
     </row>
     <row r="144" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B144" s="4">
         <v>8</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>131</v>
+        <v>72</v>
       </c>
       <c r="D144" s="12" t="s">
         <v>34</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="145" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A145" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B145" s="59"/>
       <c r="C145" s="59"/>
@@ -7722,7 +7719,7 @@
     </row>
     <row r="146" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B146" s="36" t="s">
         <v>41</v>
@@ -7734,7 +7731,7 @@
         <v>34</v>
       </c>
       <c r="E146" s="35" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F146" s="37"/>
       <c r="G146" s="2"/>
@@ -8021,7 +8018,7 @@
     </row>
     <row r="147" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>42</v>
@@ -8033,15 +8030,15 @@
         <v>34</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="148" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B148" s="36" t="s">
         <v>136</v>
-      </c>
-      <c r="B148" s="36" t="s">
-        <v>137</v>
       </c>
       <c r="C148" s="36" t="s">
         <v>8</v>
@@ -8050,7 +8047,7 @@
         <v>34</v>
       </c>
       <c r="E148" s="35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F148" s="37"/>
       <c r="G148" s="2"/>
@@ -8337,10 +8334,10 @@
     </row>
     <row r="149" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B149" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>8</v>
@@ -8349,12 +8346,12 @@
         <v>34</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="150" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A150" s="58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B150" s="59"/>
       <c r="C150" s="59"/>
@@ -8364,10 +8361,10 @@
     </row>
     <row r="151" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B151" s="36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C151" s="36" t="s">
         <v>8</v>
@@ -8376,7 +8373,7 @@
         <v>9</v>
       </c>
       <c r="E151" s="35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F151" s="37"/>
       <c r="G151" s="2"/>
@@ -8663,10 +8660,10 @@
     </row>
     <row r="152" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>8</v>
@@ -8675,24 +8672,24 @@
         <v>9</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="153" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="35" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B153" s="36">
         <v>4</v>
       </c>
       <c r="C153" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D153" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E153" s="35" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F153" s="37"/>
       <c r="G153" s="2"/>
@@ -8979,36 +8976,36 @@
     </row>
     <row r="154" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B154" s="4">
         <v>1</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D154" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="155" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B155" s="36">
         <v>100</v>
       </c>
       <c r="C155" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D155" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E155" s="35" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F155" s="37"/>
       <c r="G155" s="2"/>
@@ -9295,10 +9292,10 @@
     </row>
     <row r="156" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="35" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B156" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C156" s="36" t="s">
         <v>8</v>
@@ -9307,7 +9304,7 @@
         <v>34</v>
       </c>
       <c r="E156" s="35" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F156" s="37"/>
       <c r="G156" s="2"/>
@@ -9594,36 +9591,36 @@
     </row>
     <row r="157" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B157" s="4">
         <v>500</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D157" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="158" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B158" s="36">
         <v>4</v>
       </c>
       <c r="C158" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D158" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E158" s="35" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F158" s="37"/>
       <c r="G158" s="2"/>
@@ -9910,36 +9907,36 @@
     </row>
     <row r="159" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B159" s="4">
         <v>1</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D159" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="160" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="35" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B160" s="36">
         <v>100</v>
       </c>
       <c r="C160" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D160" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E160" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F160" s="37"/>
       <c r="G160" s="2"/>
@@ -10226,7 +10223,7 @@
     </row>
     <row r="161" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="35" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B161" s="36"/>
       <c r="C161" s="36" t="s">
@@ -10236,7 +10233,7 @@
         <v>34</v>
       </c>
       <c r="E161" s="35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F161" s="37"/>
       <c r="G161" s="2"/>
@@ -10523,36 +10520,36 @@
     </row>
     <row r="162" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B162" s="4">
         <v>500</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D162" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="163" spans="1:287" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B163" s="36">
         <v>4</v>
       </c>
       <c r="C163" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D163" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E163" s="35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F163" s="37"/>
       <c r="G163" s="2"/>
@@ -10839,7 +10836,7 @@
     </row>
     <row r="164" spans="1:287" x14ac:dyDescent="0.2">
       <c r="A164" s="61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B164" s="62"/>
       <c r="C164" s="62"/>
@@ -10849,10 +10846,10 @@
     </row>
     <row r="165" spans="1:287" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B165" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>8</v>
@@ -10861,12 +10858,12 @@
         <v>34</v>
       </c>
       <c r="E165" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="166" spans="1:287" s="35" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A166" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B166" s="36"/>
       <c r="C166" s="36" t="s">
@@ -10876,7 +10873,7 @@
         <v>34</v>
       </c>
       <c r="E166" s="37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F166" s="37"/>
       <c r="G166" s="2"/>
@@ -11236,66 +11233,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>152</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -11330,57 +11327,57 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="66" t="s">
         <v>152</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="s">
         <v>169</v>
-      </c>
-      <c r="B3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="s">
         <v>171</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" t="s">
         <v>173</v>
-      </c>
-      <c r="B6" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" t="s">
         <v>175</v>
-      </c>
-      <c r="B7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -11388,7 +11385,7 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -11396,89 +11393,89 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
         <v>179</v>
-      </c>
-      <c r="B11" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" t="s">
         <v>181</v>
-      </c>
-      <c r="B12" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" t="s">
         <v>183</v>
-      </c>
-      <c r="B13" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="27"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B15" s="28"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" t="s">
         <v>192</v>
-      </c>
-      <c r="B21" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
@@ -11486,18 +11483,18 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B24" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B25" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -11528,21 +11525,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>221</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -11552,15 +11549,15 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>224</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -11570,42 +11567,42 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -11613,7 +11610,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -11621,36 +11618,36 @@
         <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" t="s">
         <v>237</v>
-      </c>
-      <c r="B17" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18" t="s">
         <v>239</v>
-      </c>
-      <c r="B18" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20" t="s">
         <v>263</v>
-      </c>
-      <c r="B20" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -11658,68 +11655,68 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>242</v>
+      </c>
+      <c r="B22" s="30" t="s">
         <v>243</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23" t="s">
         <v>245</v>
-      </c>
-      <c r="B23" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
@@ -11734,22 +11731,22 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
@@ -11759,22 +11756,22 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
@@ -11784,37 +11781,37 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
@@ -11824,7 +11821,7 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
@@ -11834,7 +11831,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
@@ -11849,7 +11846,7 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
@@ -11882,26 +11879,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>152</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" t="s">
         <v>198</v>
-      </c>
-      <c r="B3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -11909,23 +11906,23 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -11933,23 +11930,23 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" t="s">
         <v>206</v>
-      </c>
-      <c r="B8" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" t="s">
         <v>208</v>
-      </c>
-      <c r="B9" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.25">
@@ -11957,31 +11954,31 @@
         <v>27</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" t="s">
         <v>210</v>
-      </c>
-      <c r="B11" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" t="s">
         <v>212</v>
-      </c>
-      <c r="B12" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" t="s">
         <v>214</v>
-      </c>
-      <c r="B13" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -11989,7 +11986,7 @@
         <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -11997,15 +11994,15 @@
         <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" t="s">
         <v>218</v>
-      </c>
-      <c r="B16" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -12013,7 +12010,7 @@
         <v>77</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -12021,15 +12018,15 @@
         <v>80</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -12037,31 +12034,31 @@
         <v>49</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B22" s="67" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B23" s="67" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.25">
@@ -12074,59 +12071,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FolderType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <CultureName xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <IsNotebookLocked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Invited_Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Math_Settings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Has_Leaders_Only_SectionGroup xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Member_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <Distribution_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <AppVersion xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Templates xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <NotebookType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <TeamsChannelId xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Invited_Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Owner xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <LMS_Mappings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <_activity xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100F5BD758A7F2BF742ADB9291A93682A9E" ma:contentTypeVersion="31" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0517f02299b6dbd064809d9c3f869e8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="35345429-01ed-4d83-85b9-6cc21878d784" xmlns:ns4="53f86fb7-11c0-476e-bf8b-57768422e991" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7ff6e993c77c55b2c02ebba747ae01b" ns3:_="" ns4:_="">
     <xsd:import namespace="35345429-01ed-4d83-85b9-6cc21878d784"/>
@@ -12523,7 +12467,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -12532,24 +12476,60 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D89A20-922B-4399-8A99-02ABCC3D1E33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="35345429-01ed-4d83-85b9-6cc21878d784"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="53f86fb7-11c0-476e-bf8b-57768422e991"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FolderType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <CultureName xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <IsNotebookLocked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Invited_Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Math_Settings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Has_Leaders_Only_SectionGroup xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Member_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <Distribution_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <AppVersion xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Templates xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <NotebookType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <TeamsChannelId xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Invited_Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Owner xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <LMS_Mappings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <_activity xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D716C96-A80E-4732-A5D3-9C77E88EE8CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12568,10 +12548,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E85C156E-EE0C-426A-92B3-CAF84DB17690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D89A20-922B-4399-8A99-02ABCC3D1E33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="35345429-01ed-4d83-85b9-6cc21878d784"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="53f86fb7-11c0-476e-bf8b-57768422e991"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>